<commit_message>
Atualização automática de pedidos - 30/05/2025 07:32
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -723,6 +723,46 @@
           <t>washington</t>
         </is>
       </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>REQ-006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>30/05/2025 07:32</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>R01-LA-B2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -735,7 +775,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -915,6 +955,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>REQ-006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A3ZPA-1.0-GY</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>180DN106041</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>GY</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 08:26
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -740,10 +740,8 @@
           <t>Renault</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -758,11 +756,59 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>30/05/2025 07:33</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>REQ-007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>30/05/2025 08:25</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>R01-LA-A2</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
           <t>Pendente</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -775,7 +821,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,10 +1017,8 @@
           <t>180DN106041</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+      <c r="D7" t="n">
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -982,6 +1026,32 @@
         </is>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>REQ-007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 08:46
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -786,10 +786,8 @@
           <t>Ford</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D8" t="n">
+        <v>1</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -809,6 +807,84 @@
       </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>REQ-008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>30/05/2025 08:38</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>13</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>R13-LA-A1</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REQ-009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>30/05/2025 08:46</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>R01-LA-A5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -821,7 +897,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1041,17 +1117,73 @@
           <t>0</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>REQ-008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ACOR2Z-0.5-L</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>180EX603990</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>L</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>REQ-009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>A3ZPA-1.0-BR</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>180DN106080</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>BR</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 08:59
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -862,10 +862,8 @@
           <t>Renault</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -885,6 +883,84 @@
       </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>REQ-010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>30/05/2025 08:55</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>R12-LA-A1</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>REQ-011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>30/05/2025 08:59</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>R12-LA-A1</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -897,7 +973,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1173,10 +1249,8 @@
           <t>180DN106080</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
+      <c r="D10" t="n">
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -1184,6 +1258,64 @@
         </is>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>REQ-010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ACOR2Z-0.35-GY</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>180EX606941</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>GY</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>REQ-011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ACOR2Z-0.35-GY</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>180EX606941</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>GY</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 09:02
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -938,10 +938,8 @@
           <t>Renault</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="D12" t="n">
+        <v>12</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -961,6 +959,46 @@
       </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>REQ-012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>30/05/2025 09:02</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>R12-LA-C1</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -973,7 +1011,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1305,10 +1343,8 @@
           <t>180EX606941</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>0.35</t>
-        </is>
+      <c r="D12" t="n">
+        <v>0.35</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1316,6 +1352,36 @@
         </is>
       </c>
       <c r="F12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>REQ-012</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ACOR2Z-0.5-BE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>180EX60395U</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BE</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 09:06
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -976,10 +976,8 @@
           <t>Renault</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="D13" t="n">
+        <v>12</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -999,6 +997,46 @@
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>REQ-013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>30/05/2025 09:06</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Renault</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>R12-LA-A1</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1011,7 +1049,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1371,10 +1409,8 @@
           <t>180EX60395U</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
+      <c r="D13" t="n">
+        <v>0.5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1382,6 +1418,36 @@
         </is>
       </c>
       <c r="F13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>REQ-013</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ACOR2Z-0.35-GY</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>180EX606941</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.35</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GY</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática de pedidos - 30/05/2025 09:14
</commit_message>
<xml_diff>
--- a/pedidos.xlsx
+++ b/pedidos.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1014,10 +1014,8 @@
           <t>Renault</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="D14" t="n">
+        <v>12</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1037,6 +1035,46 @@
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>REQ-014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>30/05/2025 09:14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Ford</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>R10-LA-A2</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>washington vieira</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Pendente</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1049,7 +1087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1437,17 +1475,45 @@
           <t>180EX606941</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GY</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>REQ-014</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>LMPT2A-0.35-G-R</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>180BA406965</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
         <is>
           <t>0.35</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>GY</t>
-        </is>
-      </c>
-      <c r="F14" t="n">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>G-R</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>